<commit_message>
feat: prc activacion envio correos
</commit_message>
<xml_diff>
--- a/email-branding/excel/FLUJO_MAIL_ID((Autorecovered-310929061547474723)).xlsx
+++ b/email-branding/excel/FLUJO_MAIL_ID((Autorecovered-310929061547474723)).xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\w\iconstruye-temp\email-branding\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\w\iconstruye-temp\email-branding\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{69F143C7-1A92-4635-9FF1-2952DA4B5AA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E928A03-6742-44E3-A4C0-56D900C01B8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,8 @@
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
     <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
-    <sheet name="SERVICES" sheetId="2" r:id="rId7"/>
+    <sheet name="Sheet2" sheetId="8" r:id="rId7"/>
+    <sheet name="SERVICES" sheetId="2" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6332" uniqueCount="6039">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6513" uniqueCount="6090">
   <si>
     <t>IDMAIL</t>
   </si>
@@ -18947,12 +18948,961 @@
   <si>
     <t>Maipu_NotaCreditoBuscar</t>
   </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>DISPARADOR</t>
+  </si>
+  <si>
+    <t>EnviarMailProveedor</t>
+  </si>
+  <si>
+    <t>EnviarMailCreacionBodegaSistema</t>
+  </si>
+  <si>
+    <t>EnviarMailStock</t>
+  </si>
+  <si>
+    <t>EnviarMailUsuario</t>
+  </si>
+  <si>
+    <t>EnviarMailPMEliminacionLinea</t>
+  </si>
+  <si>
+    <t>EnviarMailTransito</t>
+  </si>
+  <si>
+    <t>EnviarMailPMCancelacionLinea</t>
+  </si>
+  <si>
+    <t>EnviarMailProveedorIntegracion</t>
+  </si>
+  <si>
+    <t>EnviarMailOCCancelacion</t>
+  </si>
+  <si>
+    <t>EnviarMailProveedorPIIntegracion</t>
+  </si>
+  <si>
+    <t>EnviarMailPMPresupuestoExcedido</t>
+  </si>
+  <si>
+    <t>EnviarMailPMCancelacionPedidoCompleto</t>
+  </si>
+  <si>
+    <t>EnviarMailPptoErrorCargaPlanilla</t>
+  </si>
+  <si>
+    <t>EnviarMailAutorizacionVBFactura</t>
+  </si>
+  <si>
+    <t>EnviarMailAvisoCreacionMaterial</t>
+  </si>
+  <si>
+    <t>EnviarMailBodegaMobile</t>
+  </si>
+  <si>
+    <t>metodo</t>
+  </si>
+  <si>
+    <t>METODO</t>
+  </si>
+  <si>
+    <t>Msg_ActivaServicioClave</t>
+  </si>
+  <si>
+    <t>msg_ActivaServicioBD_TRASPASO</t>
+  </si>
+  <si>
+    <t>msg_ActivaServicioStock</t>
+  </si>
+  <si>
+    <t>msg_ActivaServicioMensajeriaProveedorIntegrado_Integracion</t>
+  </si>
+  <si>
+    <t>msg_ActivaServicioMensajeriaProveedor_integracion</t>
+  </si>
+  <si>
+    <t>msg_ActivaServicioMensajeriaProveedor</t>
+  </si>
+  <si>
+    <t>msg_ActivaServicioPPTOErrorPlanilla</t>
+  </si>
+  <si>
+    <t>msg_ActivaServicioMensajeriaPMPresupuestoExcedido</t>
+  </si>
+  <si>
+    <t>Msg_ActivaServicioPMLinea</t>
+  </si>
+  <si>
+    <t>msg_ActivaServicioMensajeriaPM_CancelarPMCompleto</t>
+  </si>
+  <si>
+    <t>msg_ActivaServicioPM_CancelarLinea</t>
+  </si>
+  <si>
+    <t>msg_ActivaServicioOC_Cancelar</t>
+  </si>
+  <si>
+    <t>msg_ActivaServicioCreacionBodegaSistema</t>
+  </si>
+  <si>
+    <t>msg_ActivaServicio_BodegaMobile</t>
+  </si>
+  <si>
+    <t>msg_ActivaServicio_CreacionMaterialDesdePendiente</t>
+  </si>
+  <si>
+    <t>msg_ActivaServicio_VBAJUSTE_FACTURA</t>
+  </si>
+  <si>
+    <t>CREATE procedure [dbo].[msg_ActivaServicio_CreacionMaterialDesdePendiente]_x000D_
+ @IdEmpresa int,        _x000D_
+ @IdPendiente int,        _x000D_
+ @idMstrItem int,_x000D_
+ @IdTipoMail int_x000D_
+AS _x000D_
+BEGIN _x000D_
+_x000D_
+DECLARE @Mensaje XML _x000D_
+_x000D_
+declare @XMLMensaje table_x000D_
+(_x000D_
+[IdEmpresa] int, _x000D_
+[IdPendiente] int, _x000D_
+[idMstrItem] int,_x000D_
+[IdTipoMail] int_x000D_
+)_x000D_
+_x000D_
+INSERT INTO @XMLMensaje _x000D_
+( _x000D_
+IdEmpresa, _x000D_
+IdPendiente, _x000D_
+idMstrItem,_x000D_
+IdTipoMail_x000D_
+) _x000D_
+VALUES ( _x000D_
+@IdEmpresa, _x000D_
+@IdPendiente, _x000D_
+@idMstrItem,_x000D_
+@IdTipoMail_x000D_
+) _x000D_
+_x000D_
+SELECT @Mensaje = ( SELECT * FROM @XMLMensaje_x000D_
+FOR XML PATH('param'), _x000D_
+TYPE _x000D_
+) ; _x000D_
+_x000D_
+select @Mensaje_x000D_
+_x000D_
+DECLARE @Handle UNIQUEIDENTIFIER ; _x000D_
+begin_x000D_
+	BEGIN DIALOG CONVERSATION @Handle FROM SERVICE CreacionMaterialDesdePendienteServ TO _x000D_
+	SERVICE 'CreacionMaterialDesdePendienteServ' ON CONTRACT [Contrato_Msg] WITH ENCRYPTION = OFF ; _x000D_
+	SEND ON CONVERSATION @Handle MESSAGE TYPE MsgIC (@Mensaje) ; _x000D_
+	return _x000D_
+end_x000D_
+end</t>
+  </si>
+  <si>
+    <t xml:space="preserve">--exec Msg_ActivaServicioClave 19,'Admin',9,'123456789'_x000D_
+CREATE procedure [dbo].[Msg_ActivaServicioClave]_x000D_
+--int idtipomail, string idusuario, int idempresa, string clave_x000D_
+@IdTipoMail int,_x000D_
+@IdUsuario varchar(35),_x000D_
+@IdEmpresa int,_x000D_
+@Clave varchar(250)_x000D_
+AS _x000D_
+BEGIN _x000D_
+_x000D_
+DECLARE @Mensaje XML _x000D_
+declare @XMLMensaje table_x000D_
+(_x000D_
+[IdTipoMail] int, _x000D_
+[IdUsuario] varchar(35), _x000D_
+[IdEmpresa] int, _x000D_
+[Clave] varchar(250)_x000D_
+)_x000D_
+_x000D_
+INSERT INTO @XMLMensaje _x000D_
+( _x000D_
+[IdTipoMail] , _x000D_
+[IdUsuario] , _x000D_
+[IdEmpresa] , _x000D_
+[Clave] _x000D_
+) _x000D_
+VALUES ( _x000D_
+@IdTipoMail ,_x000D_
+@IdUsuario,_x000D_
+@IdEmpresa ,_x000D_
+@Clave _x000D_
+) _x000D_
+_x000D_
+SELECT @Mensaje = ( SELECT * FROM @XMLMensaje_x000D_
+FOR XML PATH('param'), _x000D_
+TYPE _x000D_
+) ; _x000D_
+DECLARE @Handle UNIQUEIDENTIFIER ; _x000D_
+begin_x000D_
+	BEGIN DIALOG CONVERSATION @Handle FROM SERVICE UsrCambiaClaveServ TO _x000D_
+	SERVICE 'UsrCambiaClaveServ' ON CONTRACT [Contrato_Msg] WITH ENCRYPTION = OFF ; _x000D_
+	SEND ON CONVERSATION @Handle MESSAGE TYPE MsgIC (@Mensaje) ; _x000D_
+	return _x000D_
+end_x000D_
+end_x000D_
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-- 5_x000D_
+_x000D_
+CREATE procedure [dbo].[msg_ActivaServicioCreacionBodegaSistema]_x000D_
+@IdEmpresa int,_x000D_
+@IdOrgc int,_x000D_
+@IdBodega int,_x000D_
+@IdUsuarioDes varchar(30),_x000D_
+@IdTipoMail int_x000D_
+AS _x000D_
+BEGIN _x000D_
+_x000D_
+DECLARE @Mensaje XML _x000D_
+_x000D_
+declare @XMLMensaje table_x000D_
+(_x000D_
+[IdEmpresa] int, _x000D_
+[IdOrgc] INT, _x000D_
+[IdBodega] int, _x000D_
+[IdUsuarioDes] varchar(30),_x000D_
+[IdTipoMail] int_x000D_
+)_x000D_
+_x000D_
+INSERT INTO @XMLMensaje _x000D_
+( _x000D_
+[IdEmpresa] , _x000D_
+[IdOrgc] , _x000D_
+[IdBodega] , _x000D_
+[IdUsuarioDes] ,_x000D_
+[IdTipoMail] _x000D_
+) _x000D_
+VALUES ( _x000D_
+@IdEmpresa ,_x000D_
+@IdOrgc ,_x000D_
+@IdBodega ,_x000D_
+@IdUsuarioDes ,_x000D_
+@IdTipoMail _x000D_
+) _x000D_
+_x000D_
+SELECT @Mensaje = ( SELECT * FROM @XMLMensaje_x000D_
+FOR XML PATH('param'), _x000D_
+TYPE _x000D_
+) ; _x000D_
+_x000D_
+select @Mensaje_x000D_
+_x000D_
+DECLARE @Handle UNIQUEIDENTIFIER ; _x000D_
+begin_x000D_
+	BEGIN DIALOG CONVERSATION @Handle FROM SERVICE [BodegaCreacionBodegaSistemaServ] TO _x000D_
+	SERVICE 'BodegaCreacionBodegaSistemaServ' ON CONTRACT [Contrato_Msg] WITH ENCRYPTION = OFF ; _x000D_
+	SEND ON CONVERSATION @Handle MESSAGE TYPE MsgIC (@Mensaje) ; _x000D_
+	return _x000D_
+end_x000D_
+end_x000D_
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-- 7_x000D_
+_x000D_
+CREATE procedure [dbo].[msg_ActivaServicioMensajeriaProveedor]_x000D_
+@IdEmpresa int,_x000D_
+@IdOrgc int,_x000D_
+@Iddoc int,_x000D_
+@idempresaventa int,_x000D_
+@Idorgv int,_x000D_
+@IdUsuarioDes varchar(30),_x000D_
+@IdTipoMail int_x000D_
+AS _x000D_
+_x000D_
+BEGIN _x000D_
+_x000D_
+DECLARE @Mensaje XML _x000D_
+_x000D_
+declare @XMLMensaje table_x000D_
+(_x000D_
+[idempresa] int, _x000D_
+[idorgc] INT, _x000D_
+[iddoc] int, _x000D_
+[IdEmpresav] int, _x000D_
+[Idorgv] int, _x000D_
+[IdUsuarioDes] varchar(30),_x000D_
+[idtipomail] int_x000D_
+)_x000D_
+_x000D_
+INSERT INTO @XMLMensaje _x000D_
+( _x000D_
+[idempresa] , _x000D_
+[idorgc] , _x000D_
+[iddoc] , _x000D_
+[IdEmpresav],_x000D_
+[Idorgv],_x000D_
+[IdUsuarioDes] ,_x000D_
+[idtipomail] _x000D_
+) _x000D_
+VALUES ( _x000D_
+@IdEmpresa ,_x000D_
+@IdOrgc ,_x000D_
+@Iddoc ,_x000D_
+@idempresaventa,_x000D_
+@Idorgv,_x000D_
+@IdUsuarioDes ,_x000D_
+@IdTipoMail _x000D_
+) _x000D_
+_x000D_
+SELECT @Mensaje = ( SELECT * FROM @XMLMensaje_x000D_
+FOR XML PATH('param'), _x000D_
+TYPE _x000D_
+) ; _x000D_
+_x000D_
+select @Mensaje_x000D_
+_x000D_
+DECLARE @Handle UNIQUEIDENTIFIER ;_x000D_
+_x000D_
+if @idtipomail = 84_x000D_
+begin_x000D_
+	BEGIN DIALOG CONVERSATION @Handle FROM SERVICE [AprobacionFacturaProveedorServ] TO _x000D_
+	SERVICE 'AprobacionFacturaProveedorServ' ON CONTRACT [Contrato_Msg] WITH ENCRYPTION = OFF ; _x000D_
+	SEND ON CONVERSATION @Handle MESSAGE TYPE MsgIC (@Mensaje) ; _x000D_
+	return _x000D_
+end_x000D_
+_x000D_
+if @idtipomail in (25,26) --ct_x000D_
+begin_x000D_
+	BEGIN DIALOG CONVERSATION @Handle FROM SERVICE CotizacionPubModServ TO _x000D_
+	SERVICE 'CotizacionPubModServ' ON CONTRACT [Contrato_Msg] WITH ENCRYPTION = OFF ; _x000D_
+	SEND ON CONVERSATION @Handle MESSAGE TYPE MsgIC (@Mensaje) ; _x000D_
+	return _x000D_
+end_x000D_
+_x000D_
+if @idtipomail = 85_x000D_
+begin_x000D_
+	BEGIN DIALOG CONVERSATION @Handle FROM SERVICE [SolicitudNotaCorreccionProveedorServ] TO _x000D_
+	SERVICE 'SolicitudNotaCorreccionProveedorServ' ON CONTRACT [Contrato_Msg] WITH ENCRYPTION = OFF ; _x000D_
+	SEND ON CONVERSATION @Handle MESSAGE TYPE MsgIC (@Mensaje) ; _x000D_
+	return _x000D_
+end_x000D_
+_x000D_
+if @idtipomail = 86_x000D_
+begin_x000D_
+	BEGIN DIALOG CONVERSATION @Handle FROM SERVICE [CancelacionNotaCorreccionProveedorServ] TO _x000D_
+	SERVICE 'CancelacionNotaCorreccionProveedorServ' ON CONTRACT [Contrato_Msg] WITH ENCRYPTION = OFF ; _x000D_
+	SEND ON CONVERSATION @Handle MESSAGE TYPE MsgIC (@Mensaje) ; _x000D_
+	return _x000D_
+end_x000D_
+_x000D_
+if @idtipomail =51  -- BD_Recepciones_con_Rechazo _x000D_
+begin _x000D_
+	BEGIN DIALOG CONVERSATION @Handle FROM SERVICE FACRechazadaServ TO _x000D_
+	SERVICE 'RecepcionRechazoServ' ON CONTRACT [Contrato_Msg] WITH ENCRYPTION = OFF ; _x000D_
+	SEND ON CONVERSATION @Handle MESSAGE TYPE MsgIC (@Mensaje) ; _x000D_
+	return_x000D_
+end_x000D_
+_x000D_
+if @idtipomail =37_x000D_
+begin _x000D_
+	BEGIN DIALOG CONVERSATION @Handle FROM SERVICE OCSolicitudCancelacionServ TO _x000D_
+	SERVICE 'OCSolicitudCancelacionServ' ON CONTRACT [Contrato_Msg] WITH ENCRYPTION = OFF ; _x000D_
+	SEND ON CONVERSATION @Handle MESSAGE TYPE MsgIC (@Mensaje) ; _x000D_
+	return_x000D_
+end_x000D_
+_x000D_
+if @idtipomail in (20,42)_x000D_
+begin _x000D_
+	BEGIN DIALOG CONVERSATION @Handle FROM SERVICE OC_AvisoServ TO _x000D_
+	SERVICE 'OC_AvisoServ' ON CONTRACT [Contrato_Msg] WITH ENCRYPTION = OFF ; _x000D_
+	SEND ON CONVERSATION @Handle MESSAGE TYPE MsgIC (@Mensaje) ; _x000D_
+	return _x000D_
+end_x000D_
+_x000D_
+_x000D_
+END_x000D_
+</t>
+  </si>
+  <si>
+    <t>CREATE PROCEDURE msg_ActivaServicio_BodegaMobile
+    @IdEmpresa		INT,
+    @IdOrgc			INT,
+	@IdDoc			INT,
+	@IdUsuario		VARCHAR(30),
+	@UsuarioDestino	VARCHAR(150),
+    @IdTipoMail		INT
+AS
+    BEGIN
+        DECLARE @Mensaje XML
+        DECLARE @XMLMensaje TABLE
+            (
+                [IdEmpresa]			INT,
+                [IdOrgc]			INT,
+				[IdDoc]				INT,
+				[IdUsuario]			VARCHAR(30),
+				[UsuarioDestino]	VARCHAR(150),
+                [IdTipoMail]		INT
+            )
+        INSERT INTO @XMLMensaje
+            (
+                IdEmpresa,
+                IdOrgc,
+				IdDoc,
+				IdUsuario,
+				UsuarioDestino,
+                IdTipoMail
+            )
+        VALUES ( @IdEmpresa, @IdOrgc, @IdDoc, @IdUsuario, @UsuarioDestino, @IdTipoMail )
+        SELECT @Mensaje =
+            (
+                SELECT *
+                FROM @XMLMensaje
+                FOR XML PATH('param'), TYPE
+            )
+        --SELECT @Mensaje
+        DECLARE @Handle UNIQUEIDENTIFIER
+        BEGIN
+            BEGIN DIALOG CONVERSATION @Handle FROM SERVICE BodegaMobileServ TO 
+            SERVICE 'BodegaMobileServ' ON CONTRACT [Contrato_Msg] WITH ENCRYPTION = OFF;
+            SEND ON CONVERSATION @Handle MESSAGE TYPE MsgIC (@Mensaje)
+            RETURN
+        END
+    END</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CREATE procedure [msg_ActivaServicio_VBAJUSTE_FACTURA]  
+@IdEmpresa int,  
+@IdOrgc int,  
+@IdDoc int,  
+@IdUsuario varchar(30),  
+@IdTipoMail int  
+AS   
+BEGIN   
+DECLARE @Mensaje XML   
+declare @XMLMensaje table  
+(  
+[IdEmpresa] int,   
+[IdOrgc] INT,   
+[IdDoc] int,   
+[IdUsuario] varchar(30),  
+[IdTipoMail] int  
+)  
+INSERT INTO @XMLMensaje   
+(   
+[IdEmpresa] ,   
+[IdOrgc] ,   
+[IdDoc] ,   
+[IdUsuario] ,  
+[IdTipoMail]   
+)   
+VALUES (   
+@IdEmpresa ,  
+@IdOrgc ,  
+@IdDoc ,  
+@IdUsuario ,  
+@IdTipoMail   
+)   
+SELECT @Mensaje = ( SELECT * FROM @XMLMensaje  
+FOR XML PATH('param'),   
+TYPE   
+) ;   
+select @Mensaje  
+DECLARE @Handle UNIQUEIDENTIFIER ;   
+begin  
+ BEGIN DIALOG CONVERSATION @Handle FROM SERVICE VBAJUSTE_FACTURA_Serv TO   
+ SERVICE 'VBAJUSTE_FACTURA_Serv' ON CONTRACT [Contrato_Msg] WITH ENCRYPTION = OFF ;   
+ SEND ON CONVERSATION @Handle MESSAGE TYPE MsgIC (@Mensaje) ;   
+ return   
+end  
+end  
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CREATE procedure [dbo].[msg_ActivaServicioBD_TRASPASO]
+@IdEmpresa int,
+@IdOrgc int,
+@IdDoc int,
+@IdUsuarioDes varchar(30),
+@IdTipoMail int
+AS 
+BEGIN 
+DECLARE @Mensaje XML 
+declare @XMLMensaje table
+(
+[IdEmpresa] int, 
+[IdOrgc] INT, 
+[IdDoc] int, 
+[IdUsuarioDes] varchar(30),
+[IdTipoMail] int
+)
+INSERT INTO @XMLMensaje 
+( 
+[IdEmpresa] , 
+[IdOrgc] , 
+[IdDoc] , 
+[IdUsuarioDes] ,
+[IdTipoMail] 
+) 
+VALUES ( 
+@IdEmpresa ,
+@IdOrgc ,
+@IdDoc ,
+@IdUsuarioDes ,
+@IdTipoMail 
+) 
+SELECT @Mensaje = ( SELECT * FROM @XMLMensaje
+FOR XML PATH('param'), 
+TYPE 
+) ; 
+select @Mensaje
+DECLARE @Handle UNIQUEIDENTIFIER ; 
+begin
+	BEGIN DIALOG CONVERSATION @Handle FROM SERVICE BD_TRASPASOServ TO 
+	SERVICE 'BD_TRASPASOServ' ON CONTRACT [Contrato_Msg] WITH ENCRYPTION = OFF ; 
+	SEND ON CONVERSATION @Handle MESSAGE TYPE MsgIC (@Mensaje) ; 
+	return 
+end
+end
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+CREATE procedure [dbo].[msg_ActivaServicioMensajeriaPM_CancelarPMCompleto]
+ @IdEmpresa int,        
+ @IdOrgc int,        
+ @IdDoc int,  
+ @IdUsuarioCancelaPM varchar(30), 
+ @FechaCancelaPM varchar(10),
+ @IdUsuarioDes varchar(30), 
+ @IdTipoMail int 
+AS 
+BEGIN 
+DECLARE @Mensaje XML 
+declare @XMLMensaje table
+(
+[IdEmpresa] int, 
+[IdOrgc] INT, 
+[IdDoc] int, 
+[IdUsuarioCancelaPM] varchar(30),
+[FechaCancelaPM] varchar(10),
+[IdUsuarioDes] varchar(30),
+[IdTipoMail] int
+)
+INSERT INTO @XMLMensaje 
+( 
+[IdEmpresa] , 
+[IdOrgc] , 
+[IdDoc] , 
+[IdUsuarioCancelaPM] ,
+[FechaCancelaPM] ,
+[IdUsuarioDes] ,
+[IdTipoMail] 
+) 
+VALUES ( 
+@IdEmpresa ,
+@IdOrgc ,
+@IdDoc ,
+@IdUsuarioCancelaPM ,
+@FechaCancelaPM ,
+@IdUsuarioDes ,
+@IdTipoMail 
+) 
+SELECT @Mensaje = ( SELECT * FROM @XMLMensaje
+FOR XML PATH('param'), 
+TYPE 
+) ; 
+select @Mensaje
+DECLARE @Handle UNIQUEIDENTIFIER ; 
+begin
+	BEGIN DIALOG CONVERSATION @Handle FROM SERVICE PM_CancelarPMCompletoServ TO 
+	SERVICE 'PM_CancelarPMCompletoServ' ON CONTRACT [Contrato_Msg] WITH ENCRYPTION = OFF ; 
+	SEND ON CONVERSATION @Handle MESSAGE TYPE MsgIC (@Mensaje) ; 
+	return 
+end
+end
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+CREATE procedure [dbo].[msg_ActivaServicioMensajeriaPMPresupuestoExcedido]
+ @IdEmpresa int,        
+ @IdOrgc int,        
+ @IdDoc int,  
+ @NomUsuarioRol varchar(100), 
+ @MailUsuarioRol varchar(150),
+ @IdTipoMail int 
+AS 
+BEGIN 
+DECLARE @Mensaje XML 
+declare @XMLMensaje table
+(
+[IdEmpresa] int, 
+[IdOrgc] INT, 
+[IdDoc] int, 
+[NomUsuarioRol] varchar(100),
+[MailUsuarioRol] varchar(150),
+[IdTipoMail] int
+)
+INSERT INTO @XMLMensaje 
+( 
+[IdEmpresa] , 
+[IdOrgc] , 
+[IdDoc] , 
+[NomUsuarioRol] , 
+[MailUsuarioRol] ,
+[IdTipoMail] 
+) 
+VALUES ( 
+@IdEmpresa ,
+@IdOrgc ,
+@IdDoc ,
+@NomUsuarioRol, 
+@MailUsuarioRol,
+@IdTipoMail 
+) 
+SELECT @Mensaje = ( SELECT * FROM @XMLMensaje
+FOR XML PATH('param'), 
+TYPE 
+) ; 
+select @Mensaje
+DECLARE @Handle UNIQUEIDENTIFIER ; 
+begin
+	BEGIN DIALOG CONVERSATION @Handle FROM SERVICE PM_PresupuestoExcedidoServ TO 
+	SERVICE 'PM_PresupuestoExcedidoServ' ON CONTRACT [Contrato_Msg] WITH ENCRYPTION = OFF ; 
+	SEND ON CONVERSATION @Handle MESSAGE TYPE MsgIC (@Mensaje) ; 
+	return 
+end
+end</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CREATE procedure [dbo].[msg_ActivaServicioMensajeriaProveedor_integracion]
+(
+@Iddoc int,
+@IdTipoMail int,
+@mailAlternativo varchar(100),
+@encriptaData varchar(200)
+)as
+BEGIN 
+DECLARE @Mensaje XML 
+declare @XMLMensaje table([Iddoc] int, [IdTipoMail] int,[MailAlternativo] varchar(100),EncriptaData varchar(200))
+INSERT INTO @XMLMensaje([Iddoc] ,[IdTipoMail] ,[MailAlternativo],[EncriptaData]) 
+VALUES ( @Iddoc ,@IdTipoMail , @mailAlternativo,@encriptaData)
+SELECT @Mensaje = ( SELECT * FROM @XMLMensaje
+FOR XML PATH('param'), 
+TYPE 
+) ; 
+select @Mensaje
+DECLARE @Handle UNIQUEIDENTIFIER ;
+/*Servicio de Integracion*/
+if @idtipomail = 90
+begin
+	BEGIN DIALOG CONVERSATION @Handle FROM SERVICE [servicioMsgIntegracion] TO 
+	SERVICE 'servicioMsgIntegracion' ON CONTRACT [Contrato_Msg] WITH ENCRYPTION = OFF ; 
+	SEND ON CONVERSATION @Handle MESSAGE TYPE MsgIC (@Mensaje) ; 
+	return 
+end
+END
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">create procedure [dbo].[msg_ActivaServicioOC_Cancelar]
+ @IdEmpresa int,        
+ @IdOrgc int,        
+ @IdDoc int,  
+ @IdUsuarioCancelaOC varchar(30), 
+ @IdUsuarioDes varchar(30), 
+ @IdTipoMail int 
+AS 
+BEGIN 
+DECLARE @Mensaje XML 
+declare @XMLMensaje table
+(
+[IdEmpresa] int, 
+[IdOrgc] INT, 
+[IdDoc] int, 
+[IdUsuarioCancelaOC] varchar(30),
+[IdUsuarioDes] varchar(30),
+[IdTipoMail] int
+)
+INSERT INTO @XMLMensaje 
+( 
+[IdEmpresa] , 
+[IdOrgc] , 
+[IdDoc] , 
+[IdUsuarioCancelaOC],
+[IdUsuarioDes] ,
+[IdTipoMail] 
+) 
+VALUES ( 
+@IdEmpresa ,
+@IdOrgc ,
+@IdDoc ,
+@IdUsuarioCancelaOC,
+@IdUsuarioDes ,
+@IdTipoMail 
+) 
+SELECT @Mensaje = ( SELECT * FROM @XMLMensaje
+FOR XML PATH('param'), 
+TYPE 
+) ; 
+select @Mensaje
+DECLARE @Handle UNIQUEIDENTIFIER ; 
+begin
+	BEGIN DIALOG CONVERSATION @Handle FROM SERVICE OC_CancelarServ TO 
+	SERVICE 'OC_CancelarServ' ON CONTRACT [Contrato_Msg] WITH ENCRYPTION = OFF ; 
+	SEND ON CONVERSATION @Handle MESSAGE TYPE MsgIC (@Mensaje) ; 
+	return 
+end
+end
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CREATE procedure [dbo].[msg_ActivaServicioPM_CancelarLinea]
+ @IdEmpresa int,        
+ @IdOrgc int,        
+ @IdDoc int,  
+ @IdLinea int,  
+ @IdUsuarioCancelaPM varchar(30), 
+ @IdUsuarioDes varchar(30), 
+ @IdTipoMail int 
+AS 
+BEGIN 
+DECLARE @Mensaje XML 
+declare @XMLMensaje table
+(
+[IdEmpresa] int, 
+[IdOrgc] INT, 
+[IdDoc] int, 
+[IdLinea] int, 
+[IdUsuarioCancelaPM] varchar(30),
+[IdUsuarioDes] varchar(30),
+[IdTipoMail] int
+)
+INSERT INTO @XMLMensaje 
+( 
+[IdEmpresa] , 
+[IdOrgc] , 
+[IdDoc] , 
+[IdLinea] , 
+[IdUsuarioCancelaPM] ,
+[IdUsuarioDes] ,
+[IdTipoMail] 
+) 
+VALUES ( 
+@IdEmpresa ,
+@IdOrgc ,
+@IdDoc ,
+@IdLinea ,
+@IdUsuarioCancelaPM ,
+@IdUsuarioDes ,
+@IdTipoMail 
+) 
+SELECT @Mensaje = ( SELECT * FROM @XMLMensaje
+FOR XML PATH('param'), 
+TYPE 
+) ; 
+-- select @Mensaje
+DECLARE @Handle UNIQUEIDENTIFIER ; 
+begin
+	BEGIN DIALOG CONVERSATION @Handle FROM SERVICE PM_CancelarLineaServ TO 
+	SERVICE 'PM_CancelarLineaServ' ON CONTRACT [Contrato_Msg] WITH ENCRYPTION = OFF ; 
+	SEND ON CONVERSATION @Handle MESSAGE TYPE MsgIC (@Mensaje) ; 
+	return 
+end
+end
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+CREATE PROCEDURE [dbo].[Msg_ActivaServicioPMLinea] 
+@idempresa int,
+@idorgc int,
+@iddoc int,
+@idLinea int,
+@idtipomail int,
+@codigo varchar(250),
+@cantidad real,
+@glosa varchar(250),
+@descripcion varchar(250),
+@actor varchar(250)
+AS 
+BEGIN 
+DECLARE @Mensaje XML 
+declare @XMLMensaje table
+(
+[idempresa] int, 
+[idorgc] INT, 
+[iddoc] int, 
+[idLinea] int,
+[idtipomail] int,
+[codigo] varchar(250),
+[cantidad] real,
+[glosa] varchar(250),
+[descripcion] varchar(250),
+[actor] varchar(250)
+)
+INSERT INTO @XMLMensaje 
+( 
+[idempresa], 
+[idorgc], 
+[iddoc], 
+[idLinea],
+[idtipomail],
+[codigo],
+[cantidad],
+[glosa],
+[descripcion],
+[actor]
+) 
+VALUES ( 
+@idempresa ,
+@idorgc ,
+@iddoc ,
+@idLinea,
+@idtipomail,
+@codigo,
+@cantidad,
+@glosa,
+@descripcion,
+@actor
+) 
+SELECT @Mensaje = ( SELECT * FROM @XMLMensaje
+FOR XML PATH('param'), 
+TYPE 
+) ; 
+DECLARE @Handle UNIQUEIDENTIFIER ; 
+-- Dialog Conversation starts here 
+begin
+	BEGIN DIALOG CONVERSATION @Handle FROM SERVICE CotizacionCierreServ TO 
+	SERVICE 'PMEliminacionLineaServ' ON CONTRACT [Contrato_Msg] WITH ENCRYPTION = OFF ; 
+	SEND ON CONVERSATION @Handle MESSAGE TYPE MsgIC (@Mensaje) ;
+	SELECT * FROM @XMLMensaje 
+	return 
+END
+end
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CREATE procedure [dbo].[msg_ActivaServicioPPTOErrorPlanilla]
+ @IdEmpresa int,        
+ @IdOrgc int,        
+ @IdUsuarioDes varchar(30),
+ @NombreArchivo varchar(200),
+ @MailDestino varchar(150),
+ @Recursos varchar(max),
+ @IdTipoMail int
+AS 
+BEGIN 
+DECLARE @Mensaje XML 
+declare @XMLMensaje table
+(
+[IdEmpresa] int, 
+[IdOrgc] INT, 
+[IdUsuarioDes] varchar(30),
+[NombreArchivo] varchar(200),
+[MailDestino] varchar(150),
+[Recursos] varchar(max),
+[IdTipoMail] int
+)
+INSERT INTO @XMLMensaje 
+( 
+[IdEmpresa], 
+[IdOrgc], 
+[IdUsuarioDes],
+[NombreArchivo],
+[MailDestino],
+[Recursos],
+[IdTipoMail]
+) 
+VALUES ( 
+@IdEmpresa, 
+@IdOrgc, 
+@IdUsuarioDes,
+@NombreArchivo,
+@MailDestino,
+@Recursos,
+@IdTipoMail
+) 
+SELECT @Mensaje = ( SELECT * FROM @XMLMensaje
+FOR XML PATH('param'), 
+TYPE 
+) ; 
+select @Mensaje
+DECLARE @Handle UNIQUEIDENTIFIER ; 
+begin
+	BEGIN DIALOG CONVERSATION @Handle FROM SERVICE PPTO_ErrorPlanillaServ TO 
+	SERVICE 'PPTO_ErrorPlanillaServ' ON CONTRACT [Contrato_Msg] WITH ENCRYPTION = OFF ; 
+	SEND ON CONVERSATION @Handle MESSAGE TYPE MsgIC (@Mensaje) ; 
+	return 
+end
+end
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CREATE procedure [dbo].[msg_ActivaServicioStock]
+@IdEmpresa int,
+@IdOrgc int,
+@IdBodega int,
+@Idmstritem int,
+@Saldo real,
+@StockCritico real,
+@IdTipoMail int
+AS 
+BEGIN 
+DECLARE @Mensaje XML 
+declare @XMLMensaje table
+(
+[IdEmpresa] int, 
+[IdOrgc] INT, 
+[IdBodega] int, 
+[Idmstritem] int,
+[Saldo] real,
+[StockCritico] real,
+[IdTipoMail] int
+)
+INSERT INTO @XMLMensaje 
+( 
+[IdEmpresa] , 
+[IdOrgc] , 
+[IdBodega] , 
+[Idmstritem] ,
+[Saldo] ,
+[StockCritico] ,
+[IdTipoMail] 
+) 
+VALUES ( 
+@IdEmpresa ,
+@IdOrgc ,
+@IdBodega ,
+@Idmstritem ,
+@Saldo ,
+@StockCritico ,
+@IdTipoMail 
+) 
+SELECT @Mensaje = ( SELECT * FROM @XMLMensaje
+FOR XML PATH('param'), 
+TYPE 
+) ; 
+DECLARE @Handle UNIQUEIDENTIFIER ; 
+begin
+	BEGIN DIALOG CONVERSATION @Handle FROM SERVICE BodegaStokCriticoServ TO 
+	SERVICE 'BodegaStokCriticoServ' ON CONTRACT [Contrato_Msg] WITH ENCRYPTION = OFF ; 
+	SEND ON CONVERSATION @Handle MESSAGE TYPE MsgIC (@Mensaje) ; 
+	return 
+end
+end
+--exec msg_ActivaServicioStock 11,1412,55,910057,55,56,82
+</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -18968,16 +19918,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -18985,12 +19947,47 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -19002,12 +19999,19 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="12">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -19029,13 +20033,109 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </right>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </right>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -19054,17 +20154,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A7B0C6DF-9E34-47B5-A83C-65E8F3E9A173}" name="Table1" displayName="Table1" ref="A1:E63" totalsRowShown="0">
-  <autoFilter ref="A1:E63" xr:uid="{A7B0C6DF-9E34-47B5-A83C-65E8F3E9A173}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E63">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A7B0C6DF-9E34-47B5-A83C-65E8F3E9A173}" name="Table1" displayName="Table1" ref="A1:F63" totalsRowShown="0">
+  <autoFilter ref="A1:F63" xr:uid="{A7B0C6DF-9E34-47B5-A83C-65E8F3E9A173}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F63">
     <sortCondition ref="A1:A63"/>
   </sortState>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{C175A9A7-8453-4168-B241-14D67AC6B3E0}" name="IDMAIL" dataDxfId="5"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{C175A9A7-8453-4168-B241-14D67AC6B3E0}" name="IDMAIL" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{282737BC-3D7B-4016-BAC4-D6C147908F24}" name="DISPARADOR" dataDxfId="10"/>
     <tableColumn id="2" xr3:uid="{287241DB-818E-48AA-AE97-7386C6CDD1DA}" name="SERVICIO"/>
     <tableColumn id="3" xr3:uid="{C59A6199-68A7-4486-A567-CA6C74509075}" name="CONTRACT"/>
-    <tableColumn id="4" xr3:uid="{7DC122CA-82EA-4079-AEFD-90BAE1E93B8B}" name="QUEUE" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{1CD13091-B643-4127-B333-042215F6BD12}" name="PRC" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{7DC122CA-82EA-4079-AEFD-90BAE1E93B8B}" name="QUEUE" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{1CD13091-B643-4127-B333-042215F6BD12}" name="PRC" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -19081,12 +20182,37 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{AF8E6F50-FB8F-4941-9552-AB8E0796FA85}" name="Table4" displayName="Table4" ref="A1:B53" totalsRowShown="0">
+  <autoFilter ref="A1:B53" xr:uid="{AF8E6F50-FB8F-4941-9552-AB8E0796FA85}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B53">
+    <sortCondition descending="1" ref="B1:B53"/>
+  </sortState>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{D711674E-EA80-4B75-94F9-169E94E70EED}" name="IDMAIL" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{397D6A6E-C64A-40E6-BF15-CB8A7400074D}" name="metodo"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{F1493136-03D7-42DF-924B-6EA8C610264A}" name="Table5" displayName="Table5" ref="E1:F17" totalsRowShown="0" dataDxfId="5" tableBorderDxfId="4">
+  <autoFilter ref="E1:F17" xr:uid="{F1493136-03D7-42DF-924B-6EA8C610264A}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{229020CE-F2BD-4B74-857E-D09C89BAE00C}" name="METODO" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{CC331982-6943-4C41-BF7A-F8299C171502}" name="Column1" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A766FBAE-E278-4091-B23C-B978AB30C00B}" name="Table2" displayName="Table2" ref="A1:C30" totalsRowShown="0">
   <autoFilter ref="A1:C30" xr:uid="{A766FBAE-E278-4091-B23C-B978AB30C00B}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{CAA793B2-5EDD-4EE7-AE2B-1BF5981D2DEA}" name="SERVICIO"/>
     <tableColumn id="2" xr3:uid="{AF5802B7-35B0-4FD7-B632-D3DD5E29AC40}" name="QUEUE"/>
-    <tableColumn id="3" xr3:uid="{2D83CD3E-3B3D-4A0E-8BA2-9EFC5EF6E9F2}" name="PRC" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{2D83CD3E-3B3D-4A0E-8BA2-9EFC5EF6E9F2}" name="PRC" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -19355,1028 +20481,1218 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E63"/>
+  <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView topLeftCell="A58" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="A64" sqref="A64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="9.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.453125" customWidth="1"/>
-    <col min="4" max="4" width="27.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.453125" customWidth="1"/>
+    <col min="5" max="5" width="27.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>6040</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>20</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C2" t="s">
         <v>13</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>46</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>21</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C3" t="s">
         <v>14</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>47</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>22</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C4" t="s">
         <v>14</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>6</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>47</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>23</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C5" t="s">
         <v>15</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>6</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>50</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>24</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C6" t="s">
         <v>16</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>6</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>49</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>27</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C7" t="s">
         <v>7</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>6</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>40</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>32</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C8" t="s">
         <v>15</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>6</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>50</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>34</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C9" t="s">
         <v>15</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>6</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>50</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>35</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C10" t="s">
         <v>15</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>6</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>50</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>36</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C11" t="s">
         <v>15</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>6</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>50</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>39</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="2" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C12" t="s">
         <v>11</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>6</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>51</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>41</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="2" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C13" t="s">
         <v>11</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>6</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>51</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>42</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="2" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C14" t="s">
         <v>13</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>6</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>46</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>43</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="2" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C15" t="s">
         <v>11</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>6</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>51</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>44</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="2" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C16" t="s">
         <v>12</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>6</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>52</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>45</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="2" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C17" t="s">
         <v>11</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>6</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>51</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>46</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="2" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C18" t="s">
         <v>11</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>6</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>51</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>47</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="2" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C19" t="s">
         <v>10</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>6</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>54</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>48</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="2" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C20" t="s">
         <v>17</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>6</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>43</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>49</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="2" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C21" t="s">
         <v>18</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>6</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>42</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
         <v>50</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="2" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C22" t="s">
         <v>19</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>6</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>44</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
         <v>52</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="2" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C23" t="s">
         <v>17</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>6</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>43</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
         <v>61</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="2" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C24" t="s">
         <v>20</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>6</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>56</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
         <v>62</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="2" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C25" t="s">
         <v>20</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>6</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>56</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="2">
         <v>63</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="2" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C26" t="s">
         <v>21</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>6</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>55</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="2">
         <v>64</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="2" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C27" t="s">
         <v>23</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>6</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>58</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="2">
         <v>65</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="2" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C28" t="s">
         <v>8</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>6</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>53</v>
       </c>
-      <c r="E28" t="s">
+      <c r="F28" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="2">
         <v>66</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="2" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C29" t="s">
         <v>8</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>6</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>53</v>
       </c>
-      <c r="E29" t="s">
+      <c r="F29" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="2">
         <v>67</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="2" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C30" t="s">
         <v>9</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
         <v>6</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>41</v>
       </c>
-      <c r="E30" t="s">
+      <c r="F30" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="2">
         <v>70</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="2" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C31" t="s">
         <v>4</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>6</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>45</v>
       </c>
-      <c r="E31" t="s">
+      <c r="F31" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" s="2">
         <v>73</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="2" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C32" t="s">
         <v>4</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>6</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
         <v>45</v>
       </c>
-      <c r="E32" t="s">
+      <c r="F32" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" s="2">
         <v>74</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="2" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C33" t="s">
         <v>4</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>6</v>
       </c>
-      <c r="D33" t="s">
+      <c r="E33" t="s">
         <v>45</v>
       </c>
-      <c r="E33" t="s">
+      <c r="F33" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" s="2">
         <v>75</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="2" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C34" t="s">
         <v>4</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
         <v>6</v>
       </c>
-      <c r="D34" t="s">
+      <c r="E34" t="s">
         <v>45</v>
       </c>
-      <c r="E34" t="s">
+      <c r="F34" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" s="2">
         <v>78</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="2" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C35" t="s">
         <v>9</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
         <v>6</v>
       </c>
-      <c r="D35" t="s">
+      <c r="E35" t="s">
         <v>41</v>
       </c>
-      <c r="E35" t="s">
+      <c r="F35" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" s="2">
         <v>79</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="2" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C36" t="s">
         <v>9</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D36" t="s">
         <v>6</v>
       </c>
-      <c r="D36" t="s">
+      <c r="E36" t="s">
         <v>41</v>
       </c>
-      <c r="E36" t="s">
+      <c r="F36" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="2">
         <v>80</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="2" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C37" t="s">
         <v>28</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" s="2">
         <v>87</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="2" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C38" t="s">
         <v>24</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D38" t="s">
         <v>6</v>
       </c>
-      <c r="D38" t="s">
+      <c r="E38" t="s">
         <v>38</v>
       </c>
-      <c r="E38" t="s">
+      <c r="F38" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" s="2">
         <v>88</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="2" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C39" t="s">
         <v>25</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D39" t="s">
         <v>6</v>
       </c>
-      <c r="D39" t="s">
+      <c r="E39" t="s">
         <v>39</v>
       </c>
-      <c r="E39" t="s">
+      <c r="F39" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" s="2">
         <v>97</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="2" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C40" t="s">
         <v>4</v>
       </c>
-      <c r="C40" t="s">
+      <c r="D40" t="s">
         <v>6</v>
       </c>
-      <c r="D40" t="s">
+      <c r="E40" t="s">
         <v>45</v>
       </c>
-      <c r="E40" t="s">
+      <c r="F40" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" s="2">
         <v>98</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="2" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C41" t="s">
         <v>4</v>
       </c>
-      <c r="C41" t="s">
+      <c r="D41" t="s">
         <v>6</v>
       </c>
-      <c r="D41" t="s">
+      <c r="E41" t="s">
         <v>45</v>
       </c>
-      <c r="E41" t="s">
+      <c r="F41" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42" s="2">
         <v>99</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="2" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C42" t="s">
         <v>4</v>
       </c>
-      <c r="C42" t="s">
+      <c r="D42" t="s">
         <v>6</v>
       </c>
-      <c r="D42" t="s">
+      <c r="E42" t="s">
         <v>45</v>
       </c>
-      <c r="E42" t="s">
+      <c r="F42" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" s="2">
         <v>106</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="2" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C43" t="s">
         <v>22</v>
       </c>
-      <c r="C43" t="s">
+      <c r="D43" t="s">
         <v>6</v>
       </c>
-      <c r="D43" t="s">
+      <c r="E43" t="s">
         <v>57</v>
       </c>
-      <c r="E43" t="s">
+      <c r="F43" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" s="2">
         <v>116</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="2" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C44" t="s">
         <v>9</v>
       </c>
-      <c r="C44" t="s">
+      <c r="D44" t="s">
         <v>6</v>
       </c>
-      <c r="D44" t="s">
+      <c r="E44" t="s">
         <v>41</v>
       </c>
-      <c r="E44" t="s">
+      <c r="F44" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45" s="2">
         <v>118</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="2" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C45" t="s">
         <v>29</v>
       </c>
-      <c r="C45" t="s">
+      <c r="D45" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" s="2">
         <v>119</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="2" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C46" t="s">
         <v>29</v>
       </c>
-      <c r="C46" t="s">
+      <c r="D46" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" s="2">
         <v>120</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="2" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C47" t="s">
         <v>30</v>
       </c>
-      <c r="C47" t="s">
+      <c r="D47" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" s="2">
         <v>121</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="2" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C48" t="s">
         <v>31</v>
       </c>
-      <c r="C48" t="s">
+      <c r="D48" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49" s="2">
         <v>122</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="2" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C49" t="s">
         <v>32</v>
       </c>
-      <c r="C49" t="s">
+      <c r="D49" t="s">
         <v>6</v>
       </c>
-      <c r="D49" t="s">
+      <c r="E49" t="s">
         <v>36</v>
       </c>
-      <c r="E49" t="s">
+      <c r="F49" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50" s="2">
         <v>123</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="2" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C50" t="s">
         <v>32</v>
       </c>
-      <c r="C50" t="s">
+      <c r="D50" t="s">
         <v>6</v>
       </c>
-      <c r="D50" t="s">
+      <c r="E50" t="s">
         <v>36</v>
       </c>
-      <c r="E50" t="s">
+      <c r="F50" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" s="2">
         <v>124</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="2" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C51" t="s">
         <v>33</v>
       </c>
-      <c r="C51" t="s">
+      <c r="D51" t="s">
         <v>6</v>
       </c>
-      <c r="D51" t="s">
+      <c r="E51" t="s">
         <v>35</v>
       </c>
-      <c r="E51" t="s">
+      <c r="F51" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52" s="2">
         <v>125</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" s="2" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C52" t="s">
         <v>34</v>
       </c>
-      <c r="C52" t="s">
+      <c r="D52" t="s">
         <v>6</v>
       </c>
-      <c r="D52" t="s">
+      <c r="E52" t="s">
         <v>37</v>
       </c>
-      <c r="E52" t="s">
+      <c r="F52" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53" s="2">
         <v>126</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" s="2" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C53" t="s">
         <v>26</v>
       </c>
-      <c r="C53" t="s">
+      <c r="D53" t="s">
         <v>6</v>
       </c>
-      <c r="D53" t="s">
+      <c r="E53" t="s">
         <v>48</v>
       </c>
-      <c r="E53" t="s">
+      <c r="F53" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54" s="2">
         <v>131</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54" s="2" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C54" t="s">
         <v>27</v>
       </c>
-      <c r="C54" t="s">
+      <c r="D54" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55" s="2">
         <v>132</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="2" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C55" t="s">
         <v>27</v>
       </c>
-      <c r="C55" t="s">
+      <c r="D55" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56" s="2">
         <v>133</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="2" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C56" t="s">
         <v>27</v>
       </c>
-      <c r="C56" t="s">
+      <c r="D56" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57" s="2">
         <v>134</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" s="2" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C57" t="s">
         <v>27</v>
       </c>
-      <c r="C57" t="s">
+      <c r="D57" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58" s="2">
         <v>135</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" s="2" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C58" t="s">
         <v>27</v>
       </c>
-      <c r="C58" t="s">
+      <c r="D58" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59" s="2">
         <v>136</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59" s="2" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C59" t="s">
         <v>27</v>
       </c>
-      <c r="C59" t="s">
+      <c r="D59" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A60" s="2">
         <v>200</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B60" s="2" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C60" t="s">
         <v>14</v>
       </c>
-      <c r="C60" t="s">
+      <c r="D60" t="s">
         <v>6</v>
       </c>
-      <c r="D60" t="s">
+      <c r="E60" t="s">
         <v>47</v>
       </c>
-      <c r="E60" t="s">
+      <c r="F60" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61" s="2">
         <v>201</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B61" s="2" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C61" t="s">
         <v>20</v>
       </c>
-      <c r="C61" t="s">
+      <c r="D61" t="s">
         <v>6</v>
       </c>
-      <c r="D61" t="s">
+      <c r="E61" t="s">
         <v>56</v>
       </c>
-      <c r="E61" t="s">
+      <c r="F61" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A62" s="2">
         <v>6501</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B62" s="2" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C62" t="s">
         <v>4</v>
       </c>
-      <c r="C62" t="s">
+      <c r="D62" t="s">
         <v>6</v>
       </c>
-      <c r="D62" t="s">
+      <c r="E62" t="s">
         <v>45</v>
       </c>
-      <c r="E62" t="s">
+      <c r="F62" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A63" s="2">
         <v>6502</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B63" s="2" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C63" t="s">
         <v>4</v>
       </c>
-      <c r="C63" t="s">
+      <c r="D63" t="s">
         <v>6</v>
       </c>
-      <c r="D63" t="s">
+      <c r="E63" t="s">
         <v>45</v>
       </c>
-      <c r="E63" t="s">
+      <c r="F63" t="s">
         <v>69</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2">
+  <conditionalFormatting sqref="A2:B2 B3:B63">
     <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -50322,7 +51638,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>67</v>
       </c>
@@ -50330,7 +51646,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>66</v>
       </c>
@@ -50338,7 +51654,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>64</v>
       </c>
@@ -50346,7 +51662,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>65</v>
       </c>
@@ -50354,7 +51670,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>63</v>
       </c>
@@ -50362,7 +51678,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>62</v>
       </c>
@@ -50370,7 +51686,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>70</v>
       </c>
@@ -50378,7 +51694,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>75</v>
       </c>
@@ -50386,7 +51702,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>78</v>
       </c>
@@ -50394,7 +51710,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>77</v>
       </c>
@@ -50402,7 +51718,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>69</v>
       </c>
@@ -50410,7 +51726,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>76</v>
       </c>
@@ -50418,7 +51734,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>61</v>
       </c>
@@ -50426,7 +51742,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>59</v>
       </c>
@@ -50434,7 +51750,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>60</v>
       </c>
@@ -51206,10 +52522,713 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C897AEE2-2BE0-43FE-B719-3D812FBB1FE1}">
+  <dimension ref="A1:G53"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15.36328125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="37.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="48.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="54" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6057</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6058</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6039</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="7">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6044</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>6044</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>6059</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="7">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6044</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>6046</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>6060</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="7">
+        <v>140</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6044</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>6043</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>6061</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="7">
+        <v>141</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6044</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>6050</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>6062</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="7">
+        <v>142</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6044</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>6048</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>6063</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="7">
+        <v>143</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6044</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>6041</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>6064</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="7">
+        <v>144</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6044</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>6053</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>6065</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" s="7">
+        <v>145</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6044</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>6051</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>6066</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="7">
+        <v>146</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6044</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>6045</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>6067</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="7">
+        <v>147</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6044</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>6052</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>6068</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="7">
+        <v>148</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6044</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>6047</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>6069</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="7">
+        <v>149</v>
+      </c>
+      <c r="B13" t="s">
+        <v>6044</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>6049</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>6070</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="7">
+        <v>150</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6044</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>6042</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>6071</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" s="7">
+        <v>151</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6044</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>6056</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>6072</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" s="7">
+        <v>152</v>
+      </c>
+      <c r="B16" t="s">
+        <v>6044</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>6055</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>6073</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17" s="7">
+        <v>153</v>
+      </c>
+      <c r="B17" t="s">
+        <v>6044</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>6054</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>6074</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18" s="7">
+        <v>154</v>
+      </c>
+      <c r="B18" t="s">
+        <v>6044</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="7">
+        <v>155</v>
+      </c>
+      <c r="B19" t="s">
+        <v>6044</v>
+      </c>
+      <c r="E19" t="s">
+        <v>6072</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>6079</v>
+      </c>
+      <c r="G19" t="str">
+        <f>_xlfn.XLOOKUP(E19,Table5[Column1],Table5[Column1])</f>
+        <v>msg_ActivaServicio_BodegaMobile</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="7">
+        <v>156</v>
+      </c>
+      <c r="B20" t="s">
+        <v>6044</v>
+      </c>
+      <c r="E20" t="s">
+        <v>6073</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>6075</v>
+      </c>
+      <c r="G20" t="str">
+        <f>_xlfn.XLOOKUP(E20,Table5[Column1],Table5[Column1])</f>
+        <v>msg_ActivaServicio_CreacionMaterialDesdePendiente</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="7">
+        <v>157</v>
+      </c>
+      <c r="B21" t="s">
+        <v>6044</v>
+      </c>
+      <c r="E21" t="s">
+        <v>6074</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>6080</v>
+      </c>
+      <c r="G21" t="str">
+        <f>_xlfn.XLOOKUP(E21,Table5[Column1],Table5[Column1])</f>
+        <v>msg_ActivaServicio_VBAJUSTE_FACTURA</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="7">
+        <v>158</v>
+      </c>
+      <c r="B22" t="s">
+        <v>6044</v>
+      </c>
+      <c r="E22" t="s">
+        <v>6060</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>6081</v>
+      </c>
+      <c r="G22" t="str">
+        <f>_xlfn.XLOOKUP(E22,Table5[Column1],Table5[Column1])</f>
+        <v>msg_ActivaServicioBD_TRASPASO</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="7">
+        <v>159</v>
+      </c>
+      <c r="B23" t="s">
+        <v>6044</v>
+      </c>
+      <c r="E23" t="s">
+        <v>6059</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>6076</v>
+      </c>
+      <c r="G23" t="str">
+        <f>_xlfn.XLOOKUP(E23,Table5[Column1],Table5[Column1])</f>
+        <v>Msg_ActivaServicioClave</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="7">
+        <v>91</v>
+      </c>
+      <c r="B24" t="s">
+        <v>6046</v>
+      </c>
+      <c r="E24" t="s">
+        <v>6071</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>6077</v>
+      </c>
+      <c r="G24" t="str">
+        <f>_xlfn.XLOOKUP(E24,Table5[Column1],Table5[Column1])</f>
+        <v>msg_ActivaServicioCreacionBodegaSistema</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="7">
+        <v>82</v>
+      </c>
+      <c r="B25" t="s">
+        <v>6043</v>
+      </c>
+      <c r="E25" t="s">
+        <v>6068</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>6082</v>
+      </c>
+      <c r="G25" t="str">
+        <f>_xlfn.XLOOKUP(E25,Table5[Column1],Table5[Column1])</f>
+        <v>msg_ActivaServicioMensajeriaPM_CancelarPMCompleto</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="7">
+        <v>95</v>
+      </c>
+      <c r="B26" t="s">
+        <v>6050</v>
+      </c>
+      <c r="E26" t="s">
+        <v>6066</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>6083</v>
+      </c>
+      <c r="G26" t="str">
+        <f>_xlfn.XLOOKUP(E26,Table5[Column1],Table5[Column1])</f>
+        <v>msg_ActivaServicioMensajeriaPMPresupuestoExcedido</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="7">
+        <v>90</v>
+      </c>
+      <c r="B27" t="s">
+        <v>6048</v>
+      </c>
+      <c r="E27" t="s">
+        <v>6064</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>6078</v>
+      </c>
+      <c r="G27" t="str">
+        <f>_xlfn.XLOOKUP(E27,Table5[Column1],Table5[Column1])</f>
+        <v>msg_ActivaServicioMensajeriaProveedor</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="7">
+        <v>25</v>
+      </c>
+      <c r="B28" t="s">
+        <v>6041</v>
+      </c>
+      <c r="E28" t="s">
+        <v>6063</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>6084</v>
+      </c>
+      <c r="G28" t="str">
+        <f>_xlfn.XLOOKUP(E28,Table5[Column1],Table5[Column1])</f>
+        <v>msg_ActivaServicioMensajeriaProveedor_integracion</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="7">
+        <v>26</v>
+      </c>
+      <c r="B29" t="s">
+        <v>6041</v>
+      </c>
+      <c r="E29" t="s">
+        <v>6070</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>6085</v>
+      </c>
+      <c r="G29" t="str">
+        <f>_xlfn.XLOOKUP(E29,Table5[Column1],Table5[Column1])</f>
+        <v>msg_ActivaServicioOC_Cancelar</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="7">
+        <v>37</v>
+      </c>
+      <c r="B30" t="s">
+        <v>6041</v>
+      </c>
+      <c r="E30" t="s">
+        <v>6069</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>6086</v>
+      </c>
+      <c r="G30" t="str">
+        <f>_xlfn.XLOOKUP(E30,Table5[Column1],Table5[Column1])</f>
+        <v>msg_ActivaServicioPM_CancelarLinea</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="7">
+        <v>42</v>
+      </c>
+      <c r="B31" t="s">
+        <v>6041</v>
+      </c>
+      <c r="E31" t="s">
+        <v>6067</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>6087</v>
+      </c>
+      <c r="G31" t="str">
+        <f>_xlfn.XLOOKUP(E31,Table5[Column1],Table5[Column1])</f>
+        <v>Msg_ActivaServicioPMLinea</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="7">
+        <v>20</v>
+      </c>
+      <c r="B32" t="s">
+        <v>6041</v>
+      </c>
+      <c r="E32" t="s">
+        <v>6065</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>6088</v>
+      </c>
+      <c r="G32" t="str">
+        <f>_xlfn.XLOOKUP(E32,Table5[Column1],Table5[Column1])</f>
+        <v>msg_ActivaServicioPPTOErrorPlanilla</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="7">
+        <v>51</v>
+      </c>
+      <c r="B33" t="s">
+        <v>6041</v>
+      </c>
+      <c r="E33" t="s">
+        <v>6061</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>6089</v>
+      </c>
+      <c r="G33" t="str">
+        <f>_xlfn.XLOOKUP(E33,Table5[Column1],Table5[Column1])</f>
+        <v>msg_ActivaServicioStock</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A34" s="7">
+        <v>84</v>
+      </c>
+      <c r="B34" t="s">
+        <v>6041</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A35" s="7">
+        <v>85</v>
+      </c>
+      <c r="B35" t="s">
+        <v>6041</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A36" s="7">
+        <v>86</v>
+      </c>
+      <c r="B36" t="s">
+        <v>6041</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A37" s="7">
+        <v>104</v>
+      </c>
+      <c r="B37" t="s">
+        <v>6053</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A38" s="7">
+        <v>100</v>
+      </c>
+      <c r="B38" t="s">
+        <v>6051</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A39" s="7">
+        <v>77</v>
+      </c>
+      <c r="B39" t="s">
+        <v>6045</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A40" s="7">
+        <v>6508</v>
+      </c>
+      <c r="B40" t="s">
+        <v>6045</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A41" s="7">
+        <v>101</v>
+      </c>
+      <c r="B41" t="s">
+        <v>6052</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A42" s="7">
+        <v>93</v>
+      </c>
+      <c r="B42" t="s">
+        <v>6047</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A43" s="7">
+        <v>94</v>
+      </c>
+      <c r="B43" t="s">
+        <v>6049</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A44" s="7">
+        <v>83</v>
+      </c>
+      <c r="B44" t="s">
+        <v>6042</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A45" s="7">
+        <v>161</v>
+      </c>
+      <c r="B45" t="s">
+        <v>6056</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A46" s="7">
+        <v>162</v>
+      </c>
+      <c r="B46" t="s">
+        <v>6056</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A47" s="7">
+        <v>163</v>
+      </c>
+      <c r="B47" t="s">
+        <v>6056</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A48" s="7">
+        <v>164</v>
+      </c>
+      <c r="B48" t="s">
+        <v>6056</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A49" s="7">
+        <v>113</v>
+      </c>
+      <c r="B49" t="s">
+        <v>6055</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A50" s="7">
+        <v>6505</v>
+      </c>
+      <c r="B50" t="s">
+        <v>6055</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A51" s="7">
+        <v>6506</v>
+      </c>
+      <c r="B51" t="s">
+        <v>6055</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A52" s="7">
+        <v>6507</v>
+      </c>
+      <c r="B52" t="s">
+        <v>6055</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A53" s="7">
+        <v>108</v>
+      </c>
+      <c r="B53" t="s">
+        <v>6054</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="2">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A61F2DC-E1F6-43E8-B949-7E3B115F1D7C}">
   <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>

</xml_diff>